<commit_message>
fixed merged dataset even better
</commit_message>
<xml_diff>
--- a/data/raw_data/EconomicData.xlsx
+++ b/data/raw_data/EconomicData.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivianaluccioli/Dropbox/DSAN5100/final_project/5100_project/data/raw_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200396E7-571E-3946-839F-1F01929B20CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Economic Data" sheetId="1" r:id="rId4"/>
+    <sheet name="Economic Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -16,12 +25,6 @@
     <t>State</t>
   </si>
   <si>
-    <t>parental_leave_mandatory_ected</t>
-  </si>
-  <si>
-    <t>parental_leave_mandatory_not_yet_ected</t>
-  </si>
-  <si>
     <t>parental_leave_voluntary</t>
   </si>
   <si>
@@ -88,9 +91,6 @@
     <t>Illinois</t>
   </si>
   <si>
-    <t>India</t>
-  </si>
-  <si>
     <t>Iowa</t>
   </si>
   <si>
@@ -100,9 +100,6 @@
     <t>Kentucky</t>
   </si>
   <si>
-    <t>Louisia</t>
-  </si>
-  <si>
     <t>Maine</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t>Missouri</t>
   </si>
   <si>
-    <t>Monta</t>
-  </si>
-  <si>
     <t>Nebraska</t>
   </si>
   <si>
@@ -145,9 +139,6 @@
     <t>New York</t>
   </si>
   <si>
-    <t>North Caroli</t>
-  </si>
-  <si>
     <t>North Dakota</t>
   </si>
   <si>
@@ -166,9 +157,6 @@
     <t>Rhode Island</t>
   </si>
   <si>
-    <t>South Caroli</t>
-  </si>
-  <si>
     <t>South Dakota</t>
   </si>
   <si>
@@ -200,22 +188,45 @@
   </si>
   <si>
     <t>US</t>
+  </si>
+  <si>
+    <t>parental_leave_mandatory_enacted</t>
+  </si>
+  <si>
+    <t>parental_leave_mandatory_not_yet_enacted</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>Indiana</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -223,39 +234,43 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -445,81 +460,86 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="B2" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G2" s="1">
         <v>51.1</v>
       </c>
       <c r="H2" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="I2" s="1">
-        <v>6118.0</v>
+        <v>6118</v>
       </c>
       <c r="J2" s="1">
         <v>7201.21</v>
@@ -528,30 +548,30 @@
         <v>11.57</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G3" s="1">
         <v>60.8</v>
       </c>
       <c r="H3" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="I3" s="1">
         <v>16630.34</v>
@@ -560,65 +580,65 @@
         <v>19574.78</v>
       </c>
       <c r="K3" s="1">
-        <v>17.74</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>17.739999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1">
         <v>55.7</v>
       </c>
       <c r="H4" s="1">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1">
         <v>53.1</v>
       </c>
       <c r="H5" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="I5" s="1">
-        <v>5655.0</v>
+        <v>5655</v>
       </c>
       <c r="J5" s="1">
         <v>6656.23</v>
@@ -627,30 +647,30 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="G6" s="1">
         <v>55.3</v>
       </c>
       <c r="H6" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I6" s="1">
         <v>14422.14</v>
@@ -659,62 +679,62 @@
         <v>16975.61</v>
       </c>
       <c r="K6" s="1">
-        <v>19.06</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>19.059999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G7" s="1">
         <v>63.2</v>
       </c>
       <c r="H7" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F8" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G8" s="1">
         <v>60.6</v>
       </c>
       <c r="H8" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="I8" s="1">
         <v>15255.5</v>
@@ -726,30 +746,30 @@
         <v>15.69</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G9" s="1">
-        <v>57.0</v>
+        <v>57</v>
       </c>
       <c r="H9" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="I9" s="1">
         <v>10600.89</v>
@@ -761,94 +781,94 @@
         <v>13.85</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F10" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G10" s="1">
         <v>66.5</v>
       </c>
       <c r="H10" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C11" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D11" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F11" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G11" s="1">
         <v>54.5</v>
       </c>
       <c r="H11" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="I11" s="1">
         <v>8343.34</v>
       </c>
       <c r="J11" s="1">
-        <v>9820.54</v>
+        <v>9820.5400000000009</v>
       </c>
       <c r="K11" s="1">
         <v>14.04</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C12" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D12" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F12" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1">
         <v>55.8</v>
       </c>
       <c r="H12" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="I12" s="1">
         <v>6011.67</v>
@@ -860,30 +880,30 @@
         <v>11.12</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F13" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1">
         <v>55.6</v>
       </c>
       <c r="H13" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I13" s="1">
         <v>17999.8</v>
@@ -895,30 +915,30 @@
         <v>18.53</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D14" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F14" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G14" s="1">
         <v>57.4</v>
       </c>
       <c r="H14" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="I14" s="1">
         <v>6756.57</v>
@@ -930,30 +950,30 @@
         <v>11.47</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C15" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D15" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F15" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G15" s="1">
         <v>60.1</v>
       </c>
       <c r="H15" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I15" s="1">
         <v>9685.94</v>
@@ -965,59 +985,59 @@
         <v>14.21</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="B16" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D16" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F16" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G16" s="1">
         <v>57.6</v>
       </c>
       <c r="H16" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C17" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D17" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F17" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G17" s="1">
         <v>63.2</v>
       </c>
       <c r="H17" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="I17" s="1">
         <v>8178.27</v>
@@ -1029,30 +1049,30 @@
         <v>11.71</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C18" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D18" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F18" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1">
         <v>61.3</v>
       </c>
       <c r="H18" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="I18" s="1">
         <v>6023.43</v>
@@ -1064,30 +1084,30 @@
         <v>9.43</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C19" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D19" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F19" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G19" s="1">
         <v>52.6</v>
       </c>
       <c r="H19" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="I19" s="1">
         <v>6390.13</v>
@@ -1099,59 +1119,59 @@
         <v>12.28</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B20" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C20" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D20" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F20" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G20" s="1">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="H20" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C21" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G21" s="1">
         <v>54.9</v>
       </c>
       <c r="H21" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I21" s="1">
         <v>9636.48</v>
@@ -1163,30 +1183,30 @@
         <v>14.85</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C22" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G22" s="1">
         <v>59.3</v>
       </c>
       <c r="H22" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="I22" s="1">
         <v>11883.39</v>
@@ -1198,30 +1218,30 @@
         <v>13.48</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G23" s="1">
         <v>60.9</v>
       </c>
       <c r="H23" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="I23" s="1">
         <v>17583.43</v>
@@ -1233,30 +1253,30 @@
         <v>18.95</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B24" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C24" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D24" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F24" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G24" s="1">
         <v>54.8</v>
       </c>
       <c r="H24" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="I24" s="1">
         <v>8799.4</v>
@@ -1268,30 +1288,30 @@
         <v>14.33</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B25" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C25" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E25" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G25" s="1">
         <v>63.9</v>
       </c>
       <c r="H25" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="I25" s="1">
         <v>10603.22</v>
@@ -1303,30 +1323,30 @@
         <v>14.28</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B26" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C26" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D26" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E26" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F26" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G26" s="1">
         <v>51.1</v>
       </c>
       <c r="H26" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="I26" s="1">
         <v>3643.37</v>
@@ -1338,94 +1358,94 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B27" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C27" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D27" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F27" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G27" s="1">
         <v>57.4</v>
       </c>
       <c r="H27" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="I27" s="1">
         <v>7302.33</v>
       </c>
       <c r="J27" s="1">
-        <v>8595.22</v>
+        <v>8595.2199999999993</v>
       </c>
       <c r="K27" s="1">
         <v>10.91</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="B28" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C28" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D28" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F28" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G28" s="1">
         <v>60.8</v>
       </c>
       <c r="H28" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B29" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C29" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D29" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E29" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F29" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G29" s="1">
         <v>65.5</v>
       </c>
       <c r="H29" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I29" s="1">
         <v>8151.36</v>
@@ -1437,30 +1457,30 @@
         <v>12.29</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C30" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D30" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F30" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G30" s="1">
         <v>55.7</v>
       </c>
       <c r="H30" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="I30" s="1">
         <v>8538.4</v>
@@ -1472,30 +1492,30 @@
         <v>12.26</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B31" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C31" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D31" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F31" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="G31" s="1">
         <v>60.7</v>
       </c>
       <c r="H31" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="I31" s="1">
         <v>11261.59</v>
@@ -1507,30 +1527,30 @@
         <v>13.63</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B32" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D32" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F32" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G32" s="1">
         <v>57.5</v>
       </c>
       <c r="H32" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I32" s="1">
         <v>12595.07</v>
@@ -1542,59 +1562,59 @@
         <v>13.01</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B33" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C33" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D33" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E33" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F33" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G33" s="1">
         <v>50.5</v>
       </c>
       <c r="H33" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B34" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D34" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E34" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F34" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G34" s="1">
         <v>55.4</v>
       </c>
       <c r="H34" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="I34" s="1">
         <v>12962.59</v>
@@ -1606,97 +1626,97 @@
         <v>17.57</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B35" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C35" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D35" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E35" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F35" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G35" s="1">
         <v>56.1</v>
       </c>
       <c r="H35" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B36" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C36" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D36" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E36" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F36" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G36" s="1">
         <v>63.8</v>
       </c>
       <c r="H36" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I36" s="1">
         <v>7997.78</v>
       </c>
       <c r="J36" s="1">
-        <v>9413.8</v>
+        <v>9413.7999999999993</v>
       </c>
       <c r="K36" s="1">
         <v>10.33</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B37" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C37" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D37" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E37" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F37" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G37" s="1">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="H37" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="I37" s="1">
-        <v>9643.45</v>
+        <v>9643.4500000000007</v>
       </c>
       <c r="J37" s="1">
         <v>11350.84</v>
@@ -1705,30 +1725,30 @@
         <v>14.63</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B38" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C38" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D38" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E38" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F38" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G38" s="1">
         <v>55.9</v>
       </c>
       <c r="H38" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="I38" s="1">
         <v>7732.5</v>
@@ -1740,30 +1760,30 @@
         <v>13.32</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B39" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C39" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D39" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E39" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G39" s="1">
         <v>58.5</v>
       </c>
       <c r="H39" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="I39" s="1">
         <v>9523.09</v>
@@ -1775,30 +1795,30 @@
         <v>15.02</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B40" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C40" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D40" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E40" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F40" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G40" s="1">
         <v>57.1</v>
       </c>
       <c r="H40" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="I40" s="1">
         <v>9524.15</v>
@@ -1810,30 +1830,30 @@
         <v>13.88</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B41" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C41" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D41" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E41" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F41" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="G41" s="1">
         <v>60.6</v>
       </c>
       <c r="H41" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I41" s="1">
         <v>13749.63</v>
@@ -1845,59 +1865,59 @@
         <v>14.74</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B42" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C42" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D42" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E42" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F42" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G42" s="1">
         <v>52.1</v>
       </c>
       <c r="H42" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B43" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C43" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D43" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E43" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F43" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G43" s="1">
         <v>63.6</v>
       </c>
       <c r="H43" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="I43" s="1">
         <v>5639.65</v>
@@ -1906,33 +1926,33 @@
         <v>6638.16</v>
       </c>
       <c r="K43" s="1">
-        <v>9.21</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>9.2100000000000009</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B44" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C44" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D44" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E44" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F44" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G44" s="1">
         <v>54.2</v>
       </c>
       <c r="H44" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="I44" s="1">
         <v>7398.45</v>
@@ -1944,30 +1964,30 @@
         <v>13.51</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B45" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C45" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D45" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E45" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F45" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G45" s="1">
         <v>56.8</v>
       </c>
       <c r="H45" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="I45" s="1">
         <v>7403.17</v>
@@ -1979,33 +1999,33 @@
         <v>12.27</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B46" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C46" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D46" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E46" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F46" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G46" s="1">
         <v>59.9</v>
       </c>
       <c r="H46" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="I46" s="1">
-        <v>8705.37</v>
+        <v>8705.3700000000008</v>
       </c>
       <c r="J46" s="1">
         <v>10246.68</v>
@@ -2014,30 +2034,30 @@
         <v>12.58</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B47" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C47" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D47" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E47" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F47" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="G47" s="1">
         <v>61.3</v>
       </c>
       <c r="H47" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="I47" s="1">
         <v>11803.26</v>
@@ -2046,33 +2066,33 @@
         <v>13893.05</v>
       </c>
       <c r="K47" s="1">
-        <v>16.49</v>
-      </c>
-    </row>
-    <row r="48">
+        <v>16.489999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B48" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C48" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D48" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E48" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F48" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G48" s="1">
         <v>60.6</v>
       </c>
       <c r="H48" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I48" s="1">
         <v>9432.33</v>
@@ -2084,30 +2104,30 @@
         <v>13.23</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B49" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C49" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D49" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E49" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F49" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G49" s="1">
         <v>58.6</v>
       </c>
       <c r="H49" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="I49" s="1">
         <v>12116.99</v>
@@ -2119,30 +2139,30 @@
         <v>17.61</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B50" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C50" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D50" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E50" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F50" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G50" s="1">
         <v>49.5</v>
       </c>
       <c r="H50" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="I50" s="1">
         <v>6920.15</v>
@@ -2154,30 +2174,30 @@
         <v>12.69</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B51" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C51" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D51" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E51" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F51" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G51" s="1">
         <v>59.3</v>
       </c>
       <c r="H51" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="I51" s="1">
         <v>10164.91</v>
@@ -2189,30 +2209,30 @@
         <v>14.48</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B52" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C52" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D52" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E52" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F52" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G52" s="1">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="H52" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="I52" s="1">
         <v>7514.18</v>
@@ -2221,12 +2241,12 @@
         <v>8844.58</v>
       </c>
       <c r="K52" s="1">
-        <v>9.8</v>
-      </c>
-    </row>
-    <row r="53">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2235,13 +2255,13 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed typo in economic data column
</commit_message>
<xml_diff>
--- a/data/raw_data/EconomicData.xlsx
+++ b/data/raw_data/EconomicData.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivianaluccioli/Dropbox/DSAN5100/final_project/5100_project/data/raw_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53025B79-706C-CC41-97C8-CDB8AACD0953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Economic Data" sheetId="1" r:id="rId4"/>
+    <sheet name="Economic Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -16,12 +25,6 @@
     <t>State</t>
   </si>
   <si>
-    <t>parental_leave_mandatory_ected</t>
-  </si>
-  <si>
-    <t>parental_leave_mandatory_not_yet_ected</t>
-  </si>
-  <si>
     <t>parental_leave_voluntary</t>
   </si>
   <si>
@@ -200,22 +203,30 @@
   </si>
   <si>
     <t>US</t>
+  </si>
+  <si>
+    <t>parental_leave_mandatory_enacted</t>
+  </si>
+  <si>
+    <t>parental_leave_mandatory_not_yet_enacted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -223,39 +234,43 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -445,81 +460,86 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="B2" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G2" s="1">
         <v>51.1</v>
       </c>
       <c r="H2" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="I2" s="1">
-        <v>6118.0</v>
+        <v>6118</v>
       </c>
       <c r="J2" s="1">
         <v>7201.21</v>
@@ -528,30 +548,30 @@
         <v>11.57</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G3" s="1">
         <v>60.8</v>
       </c>
       <c r="H3" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="I3" s="1">
         <v>16630.34</v>
@@ -560,65 +580,65 @@
         <v>19574.78</v>
       </c>
       <c r="K3" s="1">
-        <v>17.74</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>17.739999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1">
         <v>55.7</v>
       </c>
       <c r="H4" s="1">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1">
         <v>53.1</v>
       </c>
       <c r="H5" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="I5" s="1">
-        <v>5655.0</v>
+        <v>5655</v>
       </c>
       <c r="J5" s="1">
         <v>6656.23</v>
@@ -627,30 +647,30 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="G6" s="1">
         <v>55.3</v>
       </c>
       <c r="H6" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I6" s="1">
         <v>14422.14</v>
@@ -659,62 +679,62 @@
         <v>16975.61</v>
       </c>
       <c r="K6" s="1">
-        <v>19.06</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>19.059999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G7" s="1">
         <v>63.2</v>
       </c>
       <c r="H7" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F8" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G8" s="1">
         <v>60.6</v>
       </c>
       <c r="H8" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="I8" s="1">
         <v>15255.5</v>
@@ -726,30 +746,30 @@
         <v>15.69</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G9" s="1">
-        <v>57.0</v>
+        <v>57</v>
       </c>
       <c r="H9" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="I9" s="1">
         <v>10600.89</v>
@@ -761,94 +781,94 @@
         <v>13.85</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F10" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G10" s="1">
         <v>66.5</v>
       </c>
       <c r="H10" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C11" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D11" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F11" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G11" s="1">
         <v>54.5</v>
       </c>
       <c r="H11" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="I11" s="1">
         <v>8343.34</v>
       </c>
       <c r="J11" s="1">
-        <v>9820.54</v>
+        <v>9820.5400000000009</v>
       </c>
       <c r="K11" s="1">
         <v>14.04</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C12" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D12" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F12" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1">
         <v>55.8</v>
       </c>
       <c r="H12" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="I12" s="1">
         <v>6011.67</v>
@@ -860,30 +880,30 @@
         <v>11.12</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F13" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1">
         <v>55.6</v>
       </c>
       <c r="H13" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I13" s="1">
         <v>17999.8</v>
@@ -895,30 +915,30 @@
         <v>18.53</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D14" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F14" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G14" s="1">
         <v>57.4</v>
       </c>
       <c r="H14" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="I14" s="1">
         <v>6756.57</v>
@@ -930,30 +950,30 @@
         <v>11.47</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C15" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D15" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F15" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G15" s="1">
         <v>60.1</v>
       </c>
       <c r="H15" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I15" s="1">
         <v>9685.94</v>
@@ -965,59 +985,59 @@
         <v>14.21</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="2" t="s">
-        <v>25</v>
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B16" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D16" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F16" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G16" s="1">
         <v>57.6</v>
       </c>
       <c r="H16" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C17" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D17" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F17" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G17" s="1">
         <v>63.2</v>
       </c>
       <c r="H17" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="I17" s="1">
         <v>8178.27</v>
@@ -1029,30 +1049,30 @@
         <v>11.71</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C18" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D18" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F18" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1">
         <v>61.3</v>
       </c>
       <c r="H18" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="I18" s="1">
         <v>6023.43</v>
@@ -1064,30 +1084,30 @@
         <v>9.43</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C19" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D19" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F19" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G19" s="1">
         <v>52.6</v>
       </c>
       <c r="H19" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="I19" s="1">
         <v>6390.13</v>
@@ -1099,59 +1119,59 @@
         <v>12.28</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="2" t="s">
-        <v>29</v>
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B20" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C20" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D20" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F20" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G20" s="1">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="H20" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C21" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G21" s="1">
         <v>54.9</v>
       </c>
       <c r="H21" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I21" s="1">
         <v>9636.48</v>
@@ -1163,30 +1183,30 @@
         <v>14.85</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C22" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G22" s="1">
         <v>59.3</v>
       </c>
       <c r="H22" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="I22" s="1">
         <v>11883.39</v>
@@ -1198,30 +1218,30 @@
         <v>13.48</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G23" s="1">
         <v>60.9</v>
       </c>
       <c r="H23" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="I23" s="1">
         <v>17583.43</v>
@@ -1233,30 +1253,30 @@
         <v>18.95</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C24" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D24" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F24" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G24" s="1">
         <v>54.8</v>
       </c>
       <c r="H24" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="I24" s="1">
         <v>8799.4</v>
@@ -1268,30 +1288,30 @@
         <v>14.33</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C25" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E25" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G25" s="1">
         <v>63.9</v>
       </c>
       <c r="H25" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="I25" s="1">
         <v>10603.22</v>
@@ -1303,30 +1323,30 @@
         <v>14.28</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C26" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D26" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E26" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F26" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G26" s="1">
         <v>51.1</v>
       </c>
       <c r="H26" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="I26" s="1">
         <v>3643.37</v>
@@ -1338,94 +1358,94 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B27" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C27" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D27" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F27" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G27" s="1">
         <v>57.4</v>
       </c>
       <c r="H27" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="I27" s="1">
         <v>7302.33</v>
       </c>
       <c r="J27" s="1">
-        <v>8595.22</v>
+        <v>8595.2199999999993</v>
       </c>
       <c r="K27" s="1">
         <v>10.91</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="2" t="s">
-        <v>37</v>
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B28" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C28" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D28" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F28" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G28" s="1">
         <v>60.8</v>
       </c>
       <c r="H28" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B29" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C29" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D29" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E29" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F29" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G29" s="1">
         <v>65.5</v>
       </c>
       <c r="H29" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I29" s="1">
         <v>8151.36</v>
@@ -1437,30 +1457,30 @@
         <v>12.29</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C30" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D30" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F30" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G30" s="1">
         <v>55.7</v>
       </c>
       <c r="H30" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="I30" s="1">
         <v>8538.4</v>
@@ -1472,30 +1492,30 @@
         <v>12.26</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B31" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C31" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D31" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F31" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="G31" s="1">
         <v>60.7</v>
       </c>
       <c r="H31" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="I31" s="1">
         <v>11261.59</v>
@@ -1507,30 +1527,30 @@
         <v>13.63</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B32" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D32" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F32" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G32" s="1">
         <v>57.5</v>
       </c>
       <c r="H32" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I32" s="1">
         <v>12595.07</v>
@@ -1542,59 +1562,59 @@
         <v>13.01</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B33" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C33" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D33" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E33" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F33" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G33" s="1">
         <v>50.5</v>
       </c>
       <c r="H33" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B34" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D34" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E34" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F34" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G34" s="1">
         <v>55.4</v>
       </c>
       <c r="H34" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="I34" s="1">
         <v>12962.59</v>
@@ -1606,97 +1626,97 @@
         <v>17.57</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="2" t="s">
-        <v>44</v>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B35" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C35" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D35" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E35" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F35" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G35" s="1">
         <v>56.1</v>
       </c>
       <c r="H35" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B36" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C36" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D36" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E36" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F36" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G36" s="1">
         <v>63.8</v>
       </c>
       <c r="H36" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I36" s="1">
         <v>7997.78</v>
       </c>
       <c r="J36" s="1">
-        <v>9413.8</v>
+        <v>9413.7999999999993</v>
       </c>
       <c r="K36" s="1">
         <v>10.33</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B37" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C37" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D37" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E37" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F37" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G37" s="1">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="H37" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="I37" s="1">
-        <v>9643.45</v>
+        <v>9643.4500000000007</v>
       </c>
       <c r="J37" s="1">
         <v>11350.84</v>
@@ -1705,30 +1725,30 @@
         <v>14.63</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B38" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C38" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D38" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E38" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F38" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G38" s="1">
         <v>55.9</v>
       </c>
       <c r="H38" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="I38" s="1">
         <v>7732.5</v>
@@ -1740,30 +1760,30 @@
         <v>13.32</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B39" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C39" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D39" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E39" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G39" s="1">
         <v>58.5</v>
       </c>
       <c r="H39" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="I39" s="1">
         <v>9523.09</v>
@@ -1775,30 +1795,30 @@
         <v>15.02</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B40" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C40" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D40" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E40" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F40" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G40" s="1">
         <v>57.1</v>
       </c>
       <c r="H40" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="I40" s="1">
         <v>9524.15</v>
@@ -1810,30 +1830,30 @@
         <v>13.88</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B41" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C41" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D41" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E41" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F41" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="G41" s="1">
         <v>60.6</v>
       </c>
       <c r="H41" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I41" s="1">
         <v>13749.63</v>
@@ -1845,59 +1865,59 @@
         <v>14.74</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="2" t="s">
-        <v>51</v>
+    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="B42" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C42" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D42" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E42" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F42" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G42" s="1">
         <v>52.1</v>
       </c>
       <c r="H42" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B43" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C43" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D43" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E43" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F43" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G43" s="1">
         <v>63.6</v>
       </c>
       <c r="H43" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="I43" s="1">
         <v>5639.65</v>
@@ -1906,33 +1926,33 @@
         <v>6638.16</v>
       </c>
       <c r="K43" s="1">
-        <v>9.21</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>9.2100000000000009</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B44" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C44" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D44" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E44" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F44" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G44" s="1">
         <v>54.2</v>
       </c>
       <c r="H44" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="I44" s="1">
         <v>7398.45</v>
@@ -1944,30 +1964,30 @@
         <v>13.51</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B45" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C45" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D45" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E45" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F45" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G45" s="1">
         <v>56.8</v>
       </c>
       <c r="H45" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="I45" s="1">
         <v>7403.17</v>
@@ -1979,33 +1999,33 @@
         <v>12.27</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B46" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C46" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D46" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E46" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F46" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G46" s="1">
         <v>59.9</v>
       </c>
       <c r="H46" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="I46" s="1">
-        <v>8705.37</v>
+        <v>8705.3700000000008</v>
       </c>
       <c r="J46" s="1">
         <v>10246.68</v>
@@ -2014,30 +2034,30 @@
         <v>12.58</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B47" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C47" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D47" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E47" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F47" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="G47" s="1">
         <v>61.3</v>
       </c>
       <c r="H47" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="I47" s="1">
         <v>11803.26</v>
@@ -2046,33 +2066,33 @@
         <v>13893.05</v>
       </c>
       <c r="K47" s="1">
-        <v>16.49</v>
-      </c>
-    </row>
-    <row r="48">
+        <v>16.489999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B48" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C48" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D48" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E48" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F48" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G48" s="1">
         <v>60.6</v>
       </c>
       <c r="H48" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I48" s="1">
         <v>9432.33</v>
@@ -2084,30 +2104,30 @@
         <v>13.23</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B49" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C49" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D49" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E49" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F49" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G49" s="1">
         <v>58.6</v>
       </c>
       <c r="H49" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="I49" s="1">
         <v>12116.99</v>
@@ -2119,30 +2139,30 @@
         <v>17.61</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B50" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C50" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D50" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E50" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F50" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G50" s="1">
         <v>49.5</v>
       </c>
       <c r="H50" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="I50" s="1">
         <v>6920.15</v>
@@ -2154,30 +2174,30 @@
         <v>12.69</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B51" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C51" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D51" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E51" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F51" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G51" s="1">
         <v>59.3</v>
       </c>
       <c r="H51" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="I51" s="1">
         <v>10164.91</v>
@@ -2189,30 +2209,30 @@
         <v>14.48</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B52" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C52" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D52" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E52" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F52" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G52" s="1">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="H52" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="I52" s="1">
         <v>7514.18</v>
@@ -2221,12 +2241,12 @@
         <v>8844.58</v>
       </c>
       <c r="K52" s="1">
-        <v>9.8</v>
-      </c>
-    </row>
-    <row r="53">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2235,13 +2255,13 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>